<commit_message>
Requires owner approval as finishe project
</commit_message>
<xml_diff>
--- a/static/media/default/resources/products.xlsx
+++ b/static/media/default/resources/products.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\x20195893\Documents\Freelance\Freelancer\block0x\westfolks\static\media\default\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ECBCEEB-A1E4-48AC-B100-AE81326B1BE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26234FEA-2C8E-46B0-B174-FC02D9D45CCA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B9EBD318-C305-4381-9B4E-C262956256F6}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>product-name</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>product-url</t>
+  </si>
+  <si>
+    <t>product-image</t>
   </si>
 </sst>
 </file>
@@ -396,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FCADEA4-2B8F-4B28-8FFD-09C893834F43}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -408,9 +411,10 @@
     <col min="2" max="2" width="23.140625" customWidth="1"/>
     <col min="3" max="3" width="24.140625" customWidth="1"/>
     <col min="4" max="4" width="25.5703125" customWidth="1"/>
+    <col min="5" max="5" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -423,6 +427,9 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>